<commit_message>
Update Greece report with new expert variables
</commit_message>
<xml_diff>
--- a/CD-valid/Outcomes/Pretest/Greece/Greece.xlsx
+++ b/CD-valid/Outcomes/Pretest/Greece/Greece.xlsx
@@ -8,13 +8,12 @@
   <sheets>
     <sheet name="time_changes" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="tps_comparisson" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="sociodem_comparisson" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="303">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -790,6 +789,39 @@
     <t xml:space="preserve">8.7: Prisons</t>
   </si>
   <si>
+    <t xml:space="preserve">PAB_freecourts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2jupoatck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How often did the government attack the judiciary’s integrity in public?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2mecenefm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the government directly or indirectly attempt to censor the print or broadcast
+media?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2meharjrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are individual journalists harassed — i.e., threatened with libel, arrested, imprisoned,
+beaten, or killed — by governmental or powerful nongovernmental actors while engaged in
+legitimate journalistic activities?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2xel_frefair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To what extent are elections free and fair?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAB_prosecutejourn</t>
+  </si>
+  <si>
     <t xml:space="preserve">CPB_freeassoc</t>
   </si>
   <si>
@@ -799,28 +831,30 @@
     <t xml:space="preserve">To what extent do state authorities respect and protect the right of peaceful assembly?</t>
   </si>
   <si>
-    <t xml:space="preserve">PAB_freecourts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2jupoatck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How often did the government attack the judiciary’s integrity in public?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COR_govt_national</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2exbribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How routinely do members of the executive (the head of state, the head of government, and cabinet ministers), or their agents, grant favors in exchange for bribes, kickbacks, or other material inducements?</t>
+    <t xml:space="preserve">CTZ_accountability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2lginvstp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the executive were engaged in unconstitutional, illegal, or unethical activity, how likely
+is it that a legislative body (perhaps a whole chamber, perhaps a committee, whether aligned
+with government or opposition) would conduct an investigation that would result in a decision
+or report that is unfavorable to the executive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3: Absence of Embezzlement and fraud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COR_govt_local</t>
   </si>
   <si>
     <t xml:space="preserve">VDM_v2exembez</t>
   </si>
   <si>
-    <t xml:space="preserve">How often do members of the executive (the head of state, the head of government, and cabinet ministers), or their agents, steal, embezzle, or misappropriate public funds or other state resources for personal or family use?</t>
+    <t xml:space="preserve">How often do members of the executive (the head of state, the head of government, and
+cabinet ministers), or their agents, steal, embezzle, or misappropriate public funds or other
+state resources for personal or family use?</t>
   </si>
   <si>
     <t xml:space="preserve">COR_parliament</t>
@@ -832,79 +866,74 @@
     <t xml:space="preserve">Do members of the legislature abuse their position for financial gain?</t>
   </si>
   <si>
-    <t xml:space="preserve">VDM_v2mecenefm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the government directly or indirectly attempt to censor the print or broadcast media?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2meharjrn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are individual journalists harassed — i.e., threatened with libel, arrested, imprisoned, beaten, or killed — by governmental or powerful nongovernmental actors while engaged in legitimate journalistic activities?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2x_freexp_altinf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To what extent does government respect press and media freedom, the freedom of ordinary people to discuss political matters at home and in the public sphere, as well as the freedom of academic and cultural expression?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2xel_frefair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To what extent are elections free and fair?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTZ_accountability_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDM_v2lginvstp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the executive were engaged in unconstitutional, illegal, or unethical activity, how likely is it that a legislative body (perhaps a whole chamber, perhaps a committee, whether aligned with government or opposition) would conduct an investigation that would result in a decision or report that is unfavorable to the executive?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sampling_plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender_female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender_male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_18-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_25-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_35-44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_45-54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_55-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZE</t>
+    <t xml:space="preserve">FIW_F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there an independent judiciary?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIS_religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIW_D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are individuals free to practice and express their religious faith or nonbelief in public and private?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIS_politics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPB_community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIW_E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there freedom of assembly?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIW_C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are safeguards against official corruption strong and effective?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROL_equality_sig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIW_F4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do laws, policies, and practices guarantee equal treatment of various segments of the population?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSE_polinfluence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2x_jucon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To what extent does the executive respect the constitution and comply with court
+rulings, and to what extent is the judiciary able to act in an independent fashion?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAB_prosecuteopp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2x_frassoc_thick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To what extent are parties, including opposition parties, allowed to form and to
+participate in elections, and to what extent are civil society organizations able to form and to operate freely?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDM_v2elffelr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taking all aspects of the pre-election period, election day, and the post-election process
+into account, would you consider subnational elections (regional and local, as previously
+identified) to be free and fair on average?</t>
   </si>
 </sst>
 </file>
@@ -5014,13 +5043,13 @@
         <v>258</v>
       </c>
       <c r="C67" t="n">
-        <v>0.461538461538462</v>
+        <v>0.375</v>
       </c>
       <c r="D67" t="s">
         <v>259</v>
       </c>
       <c r="E67" t="n">
-        <v>0.575451847051682</v>
+        <v>0.650154154940026</v>
       </c>
       <c r="F67" t="s">
         <v>118</v>
@@ -5032,16 +5061,16 @@
         <v>260</v>
       </c>
       <c r="I67" t="n">
-        <v>0.11391338551322</v>
+        <v>0.275154154940026</v>
       </c>
       <c r="J67" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="K67" t="s">
         <v>87</v>
       </c>
       <c r="L67" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="M67" t="s">
         <v>114</v>
@@ -5052,16 +5081,16 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.452380952380952</v>
+      </c>
+      <c r="D68" t="s">
         <v>261</v>
       </c>
-      <c r="C68" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="D68" t="s">
-        <v>262</v>
-      </c>
       <c r="E68" t="n">
-        <v>0.650154154940026</v>
+        <v>0.527603451343405</v>
       </c>
       <c r="F68" t="s">
         <v>118</v>
@@ -5070,19 +5099,19 @@
         <v>14</v>
       </c>
       <c r="H68" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I68" t="n">
-        <v>0.275154154940026</v>
+        <v>0.0752224989624526</v>
       </c>
       <c r="J68" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K68" t="s">
         <v>87</v>
       </c>
       <c r="L68" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="M68" t="s">
         <v>114</v>
@@ -5093,16 +5122,16 @@
         <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>264</v>
+        <v>12</v>
       </c>
       <c r="C69" t="n">
-        <v>0.72</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="D69" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E69" t="n">
-        <v>0.355191348780337</v>
+        <v>0.521990601741349</v>
       </c>
       <c r="F69" t="s">
         <v>118</v>
@@ -5111,19 +5140,19 @@
         <v>14</v>
       </c>
       <c r="H69" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I69" t="n">
-        <v>0.364808651219663</v>
+        <v>0.188657268408016</v>
       </c>
       <c r="J69" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="K69" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="L69" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="M69" t="s">
         <v>114</v>
@@ -5134,16 +5163,16 @@
         <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="C70" t="n">
-        <v>0.72</v>
+        <v>0.565217391304348</v>
       </c>
       <c r="D70" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E70" t="n">
-        <v>0.578550689177066</v>
+        <v>0.463517890772128</v>
       </c>
       <c r="F70" t="s">
         <v>118</v>
@@ -5152,19 +5181,19 @@
         <v>14</v>
       </c>
       <c r="H70" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I70" t="n">
-        <v>0.141449310822934</v>
+        <v>0.10169950053222</v>
       </c>
       <c r="J70" t="s">
         <v>86</v>
       </c>
       <c r="K70" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="L70" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="M70" t="s">
         <v>114</v>
@@ -5175,16 +5204,16 @@
         <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C71" t="n">
-        <v>0.706666666666667</v>
+        <v>0.30952380952381</v>
       </c>
       <c r="D71" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E71" t="n">
-        <v>0.488441145281018</v>
+        <v>0.521990601741349</v>
       </c>
       <c r="F71" t="s">
         <v>118</v>
@@ -5193,19 +5222,19 @@
         <v>14</v>
       </c>
       <c r="H71" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="I71" t="n">
-        <v>0.218225521385649</v>
+        <v>0.21246679221754</v>
       </c>
       <c r="J71" t="s">
         <v>86</v>
       </c>
       <c r="K71" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="L71" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="M71" t="s">
         <v>114</v>
@@ -5216,16 +5245,16 @@
         <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>268</v>
       </c>
       <c r="C72" t="n">
-        <v>0.452380952380952</v>
+        <v>0.461538461538462</v>
       </c>
       <c r="D72" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E72" t="n">
-        <v>0.527603451343405</v>
+        <v>0.575451847051682</v>
       </c>
       <c r="F72" t="s">
         <v>118</v>
@@ -5234,19 +5263,19 @@
         <v>14</v>
       </c>
       <c r="H72" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I72" t="n">
-        <v>0.0752224989624526</v>
+        <v>0.11391338551322</v>
       </c>
       <c r="J72" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K72" t="s">
         <v>87</v>
       </c>
       <c r="L72" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="M72" t="s">
         <v>114</v>
@@ -5257,16 +5286,16 @@
         <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>271</v>
       </c>
       <c r="C73" t="n">
-        <v>0.333333333333333</v>
+        <v>0.438775510204082</v>
       </c>
       <c r="D73" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E73" t="n">
-        <v>0.521990601741349</v>
+        <v>0.58516202736899</v>
       </c>
       <c r="F73" t="s">
         <v>118</v>
@@ -5275,19 +5304,19 @@
         <v>14</v>
       </c>
       <c r="H73" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I73" t="n">
-        <v>0.188657268408016</v>
+        <v>0.146386517164908</v>
       </c>
       <c r="J73" t="s">
         <v>86</v>
       </c>
       <c r="K73" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="L73" t="s">
-        <v>132</v>
+        <v>274</v>
       </c>
       <c r="M73" t="s">
         <v>114</v>
@@ -5298,16 +5327,16 @@
         <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>275</v>
       </c>
       <c r="C74" t="n">
-        <v>0.333333333333333</v>
+        <v>0.54</v>
       </c>
       <c r="D74" t="s">
         <v>276</v>
       </c>
       <c r="E74" t="n">
-        <v>0.604759305210918</v>
+        <v>0.578550689177066</v>
       </c>
       <c r="F74" t="s">
         <v>118</v>
@@ -5319,16 +5348,16 @@
         <v>277</v>
       </c>
       <c r="I74" t="n">
-        <v>0.271425971877585</v>
+        <v>0.0385506891770656</v>
       </c>
       <c r="J74" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K74" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="L74" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="M74" t="s">
         <v>114</v>
@@ -5339,16 +5368,16 @@
         <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="C75" t="n">
-        <v>0.565217391304348</v>
+        <v>0.706666666666667</v>
       </c>
       <c r="D75" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E75" t="n">
-        <v>0.463517890772128</v>
+        <v>0.488441145281018</v>
       </c>
       <c r="F75" t="s">
         <v>118</v>
@@ -5357,19 +5386,19 @@
         <v>14</v>
       </c>
       <c r="H75" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I75" t="n">
-        <v>0.10169950053222</v>
+        <v>0.218225521385649</v>
       </c>
       <c r="J75" t="s">
         <v>86</v>
       </c>
       <c r="K75" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="L75" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="M75" t="s">
         <v>114</v>
@@ -5380,19 +5409,19 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>280</v>
+        <v>32</v>
       </c>
       <c r="C76" t="n">
-        <v>0.448275862068966</v>
+        <v>0.277777777777778</v>
       </c>
       <c r="D76" t="s">
         <v>281</v>
       </c>
       <c r="E76" t="n">
-        <v>0.58516202736899</v>
+        <v>0.75</v>
       </c>
       <c r="F76" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G76" t="s">
         <v>14</v>
@@ -5401,278 +5430,430 @@
         <v>282</v>
       </c>
       <c r="I76" t="n">
-        <v>0.136886165300024</v>
+        <v>0.472222222222222</v>
       </c>
       <c r="J76" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="K76" t="s">
-        <v>220</v>
+        <v>87</v>
       </c>
       <c r="L76" t="s">
-        <v>221</v>
+        <v>88</v>
       </c>
       <c r="M76" t="s">
         <v>114</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="77">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
         <v>283</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
         <v>284</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E77" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F77" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" t="s">
         <v>285</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I77" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J77" t="s">
+        <v>86</v>
+      </c>
+      <c r="K77" t="s">
+        <v>194</v>
+      </c>
+      <c r="L77" t="s">
+        <v>199</v>
+      </c>
+      <c r="M77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" t="s">
         <v>286</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C78" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="D78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>112</v>
+      </c>
+      <c r="G78" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" t="s">
+        <v>115</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="J78" t="s">
+        <v>86</v>
+      </c>
+      <c r="K78" t="s">
+        <v>194</v>
+      </c>
+      <c r="L78" t="s">
+        <v>199</v>
+      </c>
+      <c r="M78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
         <v>287</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C79" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="D79" t="s">
         <v>288</v>
       </c>
-      <c r="C2"/>
-      <c r="D2" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>112</v>
+      </c>
+      <c r="G79" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" t="s">
         <v>289</v>
       </c>
-      <c r="C3"/>
-      <c r="D3" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="I79" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J79" t="s">
+        <v>98</v>
+      </c>
+      <c r="K79" t="s">
+        <v>194</v>
+      </c>
+      <c r="L79" t="s">
+        <v>195</v>
+      </c>
+      <c r="M79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.183673469387755</v>
+      </c>
+      <c r="D80" t="s">
         <v>290</v>
       </c>
-      <c r="C4"/>
-      <c r="D4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E80" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F80" t="s">
+        <v>112</v>
+      </c>
+      <c r="G80" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" t="s">
         <v>291</v>
       </c>
-      <c r="C5"/>
-      <c r="D5" t="n">
+      <c r="I80" t="n">
+        <v>0.316326530612245</v>
+      </c>
+      <c r="J80" t="s">
+        <v>98</v>
+      </c>
+      <c r="K80" t="s">
+        <v>148</v>
+      </c>
+      <c r="L80" t="s">
+        <v>149</v>
+      </c>
+      <c r="M80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.464285714285714</v>
+      </c>
+      <c r="D81" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F81" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" t="s">
+        <v>215</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.285714285714286</v>
+      </c>
+      <c r="J81" t="s">
+        <v>98</v>
+      </c>
+      <c r="K81" t="s">
+        <v>194</v>
+      </c>
+      <c r="L81" t="s">
+        <v>211</v>
+      </c>
+      <c r="M81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>293</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F82" t="s">
+        <v>112</v>
+      </c>
+      <c r="G82" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" t="s">
+        <v>294</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="J82" t="s">
+        <v>98</v>
+      </c>
+      <c r="K82" t="s">
+        <v>194</v>
+      </c>
+      <c r="L82" t="s">
+        <v>199</v>
+      </c>
+      <c r="M82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="n">
         <v>0.1</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>292</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D83" t="s">
         <v>293</v>
       </c>
-      <c r="C7"/>
-      <c r="D7" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="E83" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F83" t="s">
+        <v>112</v>
+      </c>
+      <c r="G83" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" t="s">
         <v>294</v>
       </c>
-      <c r="C8"/>
-      <c r="D8" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="I83" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J83" t="s">
+        <v>98</v>
+      </c>
+      <c r="K83" t="s">
+        <v>194</v>
+      </c>
+      <c r="L83" t="s">
+        <v>199</v>
+      </c>
+      <c r="M83" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
         <v>295</v>
       </c>
-      <c r="C9"/>
-      <c r="D9" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="C84" t="n">
+        <v>0.87037037037037</v>
+      </c>
+      <c r="D84" t="s">
         <v>296</v>
       </c>
-      <c r="B10" t="s">
-        <v>288</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.510666666666667</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B11" t="s">
-        <v>289</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.489333333333333</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B12" t="s">
-        <v>290</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.0766666666666667</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.155333333333333</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>296</v>
-      </c>
-      <c r="B14" t="s">
-        <v>292</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.193333333333333</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B15" t="s">
-        <v>293</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.181666666666667</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>296</v>
-      </c>
-      <c r="B16" t="s">
-        <v>294</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.146666666666667</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>296</v>
-      </c>
-      <c r="B17" t="s">
-        <v>295</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.246666666666667</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
+      <c r="E84" t="n">
+        <v>0.620373134328358</v>
+      </c>
+      <c r="F84" t="s">
+        <v>118</v>
+      </c>
+      <c r="G84" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" t="s">
+        <v>297</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.249997236042012</v>
+      </c>
+      <c r="J84" t="s">
+        <v>86</v>
+      </c>
+      <c r="K84" t="s">
+        <v>87</v>
+      </c>
+      <c r="L84" t="s">
+        <v>88</v>
+      </c>
+      <c r="M84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>298</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.346153846153846</v>
+      </c>
+      <c r="D85" t="s">
+        <v>299</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.64430607966457</v>
+      </c>
+      <c r="F85" t="s">
+        <v>118</v>
+      </c>
+      <c r="G85" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" t="s">
+        <v>300</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.298152233510724</v>
+      </c>
+      <c r="J85" t="s">
+        <v>98</v>
+      </c>
+      <c r="K85" t="s">
+        <v>87</v>
+      </c>
+      <c r="L85" t="s">
+        <v>132</v>
+      </c>
+      <c r="M85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.565217391304348</v>
+      </c>
+      <c r="D86" t="s">
+        <v>301</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.697544916081404</v>
+      </c>
+      <c r="F86" t="s">
+        <v>118</v>
+      </c>
+      <c r="G86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" t="s">
+        <v>302</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.132327524777056</v>
+      </c>
+      <c r="J86" t="s">
+        <v>86</v>
+      </c>
+      <c r="K86" t="s">
+        <v>87</v>
+      </c>
+      <c r="L86" t="s">
+        <v>106</v>
+      </c>
+      <c r="M86" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version 3 of the HTML
</commit_message>
<xml_diff>
--- a/CD-valid/Outcomes/Pretest/Greece/Greece.xlsx
+++ b/CD-valid/Outcomes/Pretest/Greece/Greece.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">pillar</t>
   </si>
   <si>
-    <t xml:space="preserve">EL</t>
+    <t xml:space="preserve">Greece</t>
   </si>
   <si>
     <t xml:space="preserve">CPA_media_freeop</t>
@@ -333,9 +333,6 @@
     <t xml:space="preserve">Type_Survey</t>
   </si>
   <si>
-    <t xml:space="preserve">Greece</t>
-  </si>
-  <si>
     <t xml:space="preserve">Special Eurobarometer 489</t>
   </si>
   <si>
@@ -345,58 +342,58 @@
     <t xml:space="preserve">Q6_3. Please tell me whether the following points need to be improved in (OUR COUNTRY)?  (3) Judges are independent and are not under the influence of politicians or economic interests</t>
   </si>
   <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROL_courtrulings_imp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPE_489_qa6_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6_5. Please tell me whether the following points need to be improved in (OUR COUNTRY)?  (5) Public authorities and politicians respect and apply court rulings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORC_govtefforts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPE_534_QA15_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Eurobarometer SP534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA15.7. Please tell whether you agree or disagree with each of the following? :-(NATIONALITY) Government efforts to combat corruption are effective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03: Independent Oversight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORC_impartial_measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPE_534_QA15_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA15.13. Please tell whether you agree or disagree with each of the following? :-In (OUR COUNTRY) measures against corruption are applied impartially and without ulterior motives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Eurobarometer 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QB1.4 In the context of elections in Europe, how concerned or not are you about the possibility of each of the following events?:-People being pressured into voting a particular way (M)</t>
+  </si>
+  <si>
     <t xml:space="preserve">yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROL_courtrulings_imp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPE_489_qa6_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q6_5. Please tell me whether the following points need to be improved in (OUR COUNTRY)?  (5) Public authorities and politicians respect and apply court rulings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORC_govtefforts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPE_534_QA15_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Eurobarometer SP534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA15.7. Please tell whether you agree or disagree with each of the following? :-(NATIONALITY) Government efforts to combat corruption are effective</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03: Independent Oversight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORC_impartial_measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPE_534_QA15_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA15.13. Please tell whether you agree or disagree with each of the following? :-In (OUR COUNTRY) measures against corruption are applied impartially and without ulterior motives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Eurobarometer 507</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QB1.4 In the context of elections in Europe, how concerned or not are you about the possibility of each of the following events?:-People being pressured into voting a particular way (M)</t>
   </si>
   <si>
     <t xml:space="preserve">Special Eurobarometer EB043EP</t>
@@ -1346,7 +1343,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00397177890892636</v>
+        <v>0.00397177890892635</v>
       </c>
       <c r="D3" t="n">
         <v>0.565217391304348</v>
@@ -1384,7 +1381,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00397177890892636</v>
+        <v>0.00397177890892635</v>
       </c>
       <c r="D4" t="n">
         <v>0.565217391304348</v>
@@ -1498,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0129536940091125</v>
+        <v>0.0129536940091124</v>
       </c>
       <c r="D7" t="n">
         <v>0.5</v>
@@ -1574,7 +1571,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="n">
-        <v>0.000121667036916467</v>
+        <v>0.000121667036916466</v>
       </c>
       <c r="D9" t="n">
         <v>0.185185185185185</v>
@@ -1612,7 +1609,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="n">
-        <v>0.00812254429243949</v>
+        <v>0.00812254429243946</v>
       </c>
       <c r="D10" t="n">
         <v>0.438775510204082</v>
@@ -1650,7 +1647,7 @@
         <v>42</v>
       </c>
       <c r="C11" t="n">
-        <v>0.172694300044938</v>
+        <v>0.172694300044939</v>
       </c>
       <c r="D11" t="n">
         <v>0.293333333333333</v>
@@ -1802,16 +1799,16 @@
         <v>48</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0000000000286923442875393</v>
+        <v>0.971825276123052</v>
       </c>
       <c r="D15" t="n">
-        <v>0.277777777777778</v>
+        <v>0.722222222222222</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.72496984318456</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
@@ -1840,7 +1837,7 @@
         <v>50</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0000665204768798141</v>
+        <v>0.0000665204768798146</v>
       </c>
       <c r="D16" t="n">
         <v>0.38</v>
@@ -1954,7 +1951,7 @@
         <v>58</v>
       </c>
       <c r="C19" t="n">
-        <v>0.00000000000000000521326609574465</v>
+        <v>0.00000000000000000521326609574477</v>
       </c>
       <c r="D19" t="n">
         <v>0.111111111111111</v>
@@ -1992,7 +1989,7 @@
         <v>59</v>
       </c>
       <c r="C20" t="n">
-        <v>0.00000678165475469565</v>
+        <v>0.00000678165475469558</v>
       </c>
       <c r="D20" t="n">
         <v>0.0952380952380952</v>
@@ -2030,7 +2027,7 @@
         <v>60</v>
       </c>
       <c r="C21" t="n">
-        <v>0.89508471760805</v>
+        <v>0.895084717608051</v>
       </c>
       <c r="D21" t="n">
         <v>0.435897435897436</v>
@@ -2182,7 +2179,7 @@
         <v>32</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0129536940091125</v>
+        <v>0.0129536940091124</v>
       </c>
       <c r="D25" t="n">
         <v>0.5</v>
@@ -2486,7 +2483,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0129536940091125</v>
+        <v>0.0129536940091124</v>
       </c>
       <c r="D33" t="n">
         <v>0.5</v>
@@ -2524,7 +2521,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0129536940091125</v>
+        <v>0.0129536940091124</v>
       </c>
       <c r="D34" t="n">
         <v>0.5</v>
@@ -2600,7 +2597,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="n">
-        <v>0.00000477666054661017</v>
+        <v>0.00000477666054661019</v>
       </c>
       <c r="D36" t="n">
         <v>0.128205128205128</v>
@@ -2752,7 +2749,7 @@
         <v>72</v>
       </c>
       <c r="C40" t="n">
-        <v>0.00678769921219618</v>
+        <v>0.0067876992121962</v>
       </c>
       <c r="D40" t="n">
         <v>0.30952380952381</v>
@@ -2828,7 +2825,7 @@
         <v>78</v>
       </c>
       <c r="C42" t="n">
-        <v>0.000679289368248204</v>
+        <v>0.000679289368248202</v>
       </c>
       <c r="D42" t="n">
         <v>0.566666666666667</v>
@@ -2866,7 +2863,7 @@
         <v>37</v>
       </c>
       <c r="C43" t="n">
-        <v>0.000121667036916467</v>
+        <v>0.000121667036916466</v>
       </c>
       <c r="D43" t="n">
         <v>0.185185185185185</v>
@@ -2904,7 +2901,7 @@
         <v>78</v>
       </c>
       <c r="C44" t="n">
-        <v>0.000679289368248204</v>
+        <v>0.000679289368248202</v>
       </c>
       <c r="D44" t="n">
         <v>0.566666666666667</v>
@@ -2980,7 +2977,7 @@
         <v>86</v>
       </c>
       <c r="C46" t="n">
-        <v>0.364113900122292</v>
+        <v>0.364113900122293</v>
       </c>
       <c r="D46" t="n">
         <v>0.402298850574713</v>
@@ -3094,7 +3091,7 @@
         <v>37</v>
       </c>
       <c r="C49" t="n">
-        <v>0.000121667036916467</v>
+        <v>0.000121667036916466</v>
       </c>
       <c r="D49" t="n">
         <v>0.185185185185185</v>
@@ -3181,7 +3178,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
@@ -3196,19 +3193,19 @@
         <v>0.135135135135135</v>
       </c>
       <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
         <v>107</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
       </c>
       <c r="I2" t="n">
         <v>0.142642642642643</v>
       </c>
       <c r="J2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -3217,39 +3214,39 @@
         <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="n">
         <v>0.18</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" t="n">
         <v>0.143283582089552</v>
       </c>
       <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
         <v>107</v>
       </c>
-      <c r="G3" t="s">
-        <v>108</v>
-      </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I3" t="n">
         <v>0.0367164179104477</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
@@ -3258,94 +3255,94 @@
         <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" t="n">
         <v>0.183673469387755</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E4" t="n">
         <v>0.717871485943775</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I4" t="n">
         <v>0.53419801655602</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" t="n">
         <v>0.13</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" t="n">
         <v>0.756239316239316</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I5" t="n">
         <v>0.626239316239316</v>
       </c>
       <c r="J5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -3360,19 +3357,19 @@
         <v>0.437233693870862</v>
       </c>
       <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
         <v>125</v>
-      </c>
-      <c r="G6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" t="s">
-        <v>127</v>
       </c>
       <c r="I6" t="n">
         <v>0.271099639462471</v>
       </c>
       <c r="J6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
@@ -3381,12 +3378,12 @@
         <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -3401,19 +3398,19 @@
         <v>0.561066126855601</v>
       </c>
       <c r="F7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
         <v>128</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>129</v>
       </c>
       <c r="I7" t="n">
         <v>0.00415126444874725</v>
       </c>
       <c r="J7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K7" t="s">
         <v>20</v>
@@ -3422,12 +3419,12 @@
         <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -3442,19 +3439,19 @@
         <v>0.2624750499002</v>
       </c>
       <c r="F8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="G8" t="s">
-        <v>108</v>
-      </c>
       <c r="H8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I8" t="n">
         <v>0.0708582834331337</v>
       </c>
       <c r="J8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -3463,12 +3460,12 @@
         <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -3483,19 +3480,19 @@
         <v>0.297948717948718</v>
       </c>
       <c r="F9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" t="s">
         <v>107</v>
       </c>
-      <c r="G9" t="s">
-        <v>108</v>
-      </c>
       <c r="H9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I9" t="n">
         <v>0.125128205128205</v>
       </c>
       <c r="J9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -3504,12 +3501,12 @@
         <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -3524,19 +3521,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
         <v>132</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>133</v>
       </c>
       <c r="I10" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="J10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -3545,12 +3542,12 @@
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -3565,19 +3562,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I11" t="n">
         <v>0.5</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K11" t="s">
         <v>20</v>
@@ -3586,244 +3583,244 @@
         <v>19</v>
       </c>
       <c r="M11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="n">
         <v>0.647058823529412</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E12" t="n">
         <v>0.572388727802349</v>
       </c>
       <c r="F12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
         <v>138</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>139</v>
       </c>
       <c r="I12" t="n">
         <v>0.0746700957270627</v>
       </c>
       <c r="J12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K12" t="s">
         <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" t="n">
         <v>0.303571428571429</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" t="n">
         <v>0.592229746803457</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I13" t="n">
         <v>0.288658318232028</v>
       </c>
       <c r="J13" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K13" t="s">
         <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" t="n">
         <v>0.222222222222222</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14" t="n">
         <v>0.451485148514851</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I14" t="n">
         <v>0.229262926292629</v>
       </c>
       <c r="J14" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K14" t="s">
         <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="n">
         <v>0.452380952380952</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" t="n">
         <v>0.569870273409605</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I15" t="n">
         <v>0.117489321028652</v>
       </c>
       <c r="J15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K15" t="s">
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" t="n">
         <v>0.275</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E16" t="n">
         <v>0.326857142857143</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I16" t="n">
         <v>0.0518571428571428</v>
       </c>
       <c r="J16" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K16" t="s">
         <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" t="n">
         <v>0.13</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E17" t="n">
         <v>0.0816023738872404</v>
       </c>
       <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
         <v>107</v>
       </c>
-      <c r="G17" t="s">
-        <v>108</v>
-      </c>
       <c r="H17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0483976261127596</v>
+        <v>0.0483976261127597</v>
       </c>
       <c r="J17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K17" t="s">
         <v>20</v>
@@ -3832,135 +3829,135 @@
         <v>41</v>
       </c>
       <c r="M17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" t="n">
         <v>0.469135802469136</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E18" t="n">
         <v>0.455615942028986</v>
       </c>
       <c r="F18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" t="s">
+        <v>124</v>
+      </c>
+      <c r="H18" t="s">
         <v>161</v>
-      </c>
-      <c r="G18" t="s">
-        <v>126</v>
-      </c>
-      <c r="H18" t="s">
-        <v>162</v>
       </c>
       <c r="I18" t="n">
         <v>0.0135198604401502</v>
       </c>
       <c r="J18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K18" t="s">
         <v>20</v>
       </c>
       <c r="L18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" t="n">
         <v>0.360544217687075</v>
       </c>
       <c r="D19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4619708994709</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
         <v>165</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.461970899470899</v>
-      </c>
-      <c r="F19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" t="s">
-        <v>166</v>
       </c>
       <c r="I19" t="n">
         <v>0.101426681783825</v>
       </c>
       <c r="J19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K19" t="s">
         <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" t="n">
         <v>0.244897959183673</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" t="n">
         <v>0.285678137651822</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G20" t="s">
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I20" t="n">
         <v>0.0407801784681484</v>
       </c>
       <c r="J20" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K20" t="s">
         <v>44</v>
       </c>
       <c r="L20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
@@ -3975,183 +3972,183 @@
         <v>0.85982905982906</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G21" t="s">
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I21" t="n">
         <v>0.137606837606838</v>
       </c>
       <c r="J21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K21" t="s">
         <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" t="n">
         <v>0.970629370629371</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I22" t="n">
         <v>0.0293706293706294</v>
       </c>
       <c r="J22" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K22" t="s">
         <v>44</v>
       </c>
       <c r="L22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" t="n">
         <v>0.11</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E23" t="n">
         <v>0.092850049652433</v>
       </c>
       <c r="F23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" t="s">
         <v>107</v>
       </c>
-      <c r="G23" t="s">
-        <v>108</v>
-      </c>
       <c r="H23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I23" t="n">
-        <v>0.017149950347567</v>
+        <v>0.0171499503475671</v>
       </c>
       <c r="J23" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K23" t="s">
         <v>44</v>
       </c>
       <c r="L23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C24" t="n">
         <v>0.393617021276596</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E24" t="n">
         <v>0.309134287661895</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G24" t="s">
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0844827336147008</v>
+        <v>0.0844827336147007</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K24" t="s">
         <v>44</v>
       </c>
       <c r="L24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C25" t="n">
         <v>0.125</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E25" t="n">
         <v>0.753760055963624</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G25" t="s">
         <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I25" t="n">
         <v>0.628760055963624</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K25" t="s">
         <v>53</v>
@@ -4160,39 +4157,39 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C26" t="n">
         <v>0.374149659863946</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E26" t="n">
         <v>0.684210526315789</v>
       </c>
       <c r="F26" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" t="s">
         <v>187</v>
-      </c>
-      <c r="G26" t="s">
-        <v>108</v>
-      </c>
-      <c r="H26" t="s">
-        <v>188</v>
       </c>
       <c r="I26" t="n">
         <v>0.310060866451844</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K26" t="s">
         <v>53</v>
@@ -4201,39 +4198,39 @@
         <v>57</v>
       </c>
       <c r="M26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" t="n">
         <v>0.388888888888889</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E27" t="n">
         <v>0.544444444444445</v>
       </c>
       <c r="F27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I27" t="n">
         <v>0.155555555555556</v>
       </c>
       <c r="J27" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K27" t="s">
         <v>53</v>
@@ -4242,39 +4239,39 @@
         <v>57</v>
       </c>
       <c r="M27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C28" t="n">
         <v>0.588652482269504</v>
       </c>
       <c r="D28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" t="n">
         <v>0.72</v>
       </c>
       <c r="F28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I28" t="n">
         <v>0.131347517730496</v>
       </c>
       <c r="J28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K28" t="s">
         <v>53</v>
@@ -4283,39 +4280,39 @@
         <v>57</v>
       </c>
       <c r="M28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C29" t="n">
         <v>0.274074074074074</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E29" t="n">
         <v>0.488636363636364</v>
       </c>
       <c r="F29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I29" t="n">
         <v>0.21456228956229</v>
       </c>
       <c r="J29" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K29" t="s">
         <v>53</v>
@@ -4324,12 +4321,12 @@
         <v>57</v>
       </c>
       <c r="M29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -4344,19 +4341,19 @@
         <v>0.2624750499002</v>
       </c>
       <c r="F30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" t="s">
         <v>107</v>
       </c>
-      <c r="G30" t="s">
-        <v>108</v>
-      </c>
       <c r="H30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I30" t="n">
         <v>0.0708582834331337</v>
       </c>
       <c r="J30" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K30" t="s">
         <v>53</v>
@@ -4365,12 +4362,12 @@
         <v>52</v>
       </c>
       <c r="M30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -4385,19 +4382,19 @@
         <v>0.297948717948718</v>
       </c>
       <c r="F31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" t="s">
         <v>107</v>
       </c>
-      <c r="G31" t="s">
-        <v>108</v>
-      </c>
       <c r="H31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I31" t="n">
         <v>0.125128205128205</v>
       </c>
       <c r="J31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K31" t="s">
         <v>53</v>
@@ -4406,12 +4403,12 @@
         <v>52</v>
       </c>
       <c r="M31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -4426,19 +4423,19 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" t="s">
         <v>132</v>
-      </c>
-      <c r="G32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" t="s">
-        <v>133</v>
       </c>
       <c r="I32" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="J32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K32" t="s">
         <v>53</v>
@@ -4447,12 +4444,12 @@
         <v>52</v>
       </c>
       <c r="M32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -4467,19 +4464,19 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G33" t="s">
         <v>16</v>
       </c>
       <c r="H33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I33" t="n">
         <v>0.5</v>
       </c>
       <c r="J33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K33" t="s">
         <v>53</v>
@@ -4488,39 +4485,39 @@
         <v>52</v>
       </c>
       <c r="M33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C34" t="n">
         <v>0.125</v>
       </c>
       <c r="D34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E34" t="n">
         <v>0.10018018018018</v>
       </c>
       <c r="F34" t="s">
+        <v>199</v>
+      </c>
+      <c r="G34" t="s">
         <v>200</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>201</v>
-      </c>
-      <c r="H34" t="s">
-        <v>202</v>
       </c>
       <c r="I34" t="n">
         <v>0.0248198198198198</v>
       </c>
       <c r="J34" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K34" t="s">
         <v>53</v>
@@ -4529,39 +4526,39 @@
         <v>52</v>
       </c>
       <c r="M34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C35" t="n">
         <v>0.208333333333333</v>
       </c>
       <c r="D35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E35" t="n">
         <v>0.0825522710886806</v>
       </c>
       <c r="F35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" t="s">
         <v>200</v>
       </c>
-      <c r="G35" t="s">
-        <v>201</v>
-      </c>
       <c r="H35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I35" t="n">
         <v>0.125781062244653</v>
       </c>
       <c r="J35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K35" t="s">
         <v>53</v>
@@ -4570,39 +4567,39 @@
         <v>52</v>
       </c>
       <c r="M35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C36" t="n">
         <v>0.28</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E36" t="n">
         <v>0.428602227811714</v>
       </c>
       <c r="F36" t="s">
+        <v>199</v>
+      </c>
+      <c r="G36" t="s">
         <v>200</v>
       </c>
-      <c r="G36" t="s">
-        <v>201</v>
-      </c>
       <c r="H36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I36" t="n">
         <v>0.148602227811714</v>
       </c>
       <c r="J36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K36" t="s">
         <v>53</v>
@@ -4611,12 +4608,12 @@
         <v>52</v>
       </c>
       <c r="M36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -4631,19 +4628,19 @@
         <v>0.674017155110793</v>
       </c>
       <c r="F37" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" t="s">
         <v>200</v>
       </c>
-      <c r="G37" t="s">
-        <v>201</v>
-      </c>
       <c r="H37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I37" t="n">
         <v>0.294017155110793</v>
       </c>
       <c r="J37" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K37" t="s">
         <v>53</v>
@@ -4652,12 +4649,12 @@
         <v>52</v>
       </c>
       <c r="M37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
@@ -4672,19 +4669,19 @@
         <v>0.351328068916009</v>
       </c>
       <c r="F38" t="s">
+        <v>199</v>
+      </c>
+      <c r="G38" t="s">
         <v>200</v>
       </c>
-      <c r="G38" t="s">
-        <v>201</v>
-      </c>
       <c r="H38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I38" t="n">
         <v>0.171328068916009</v>
       </c>
       <c r="J38" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K38" t="s">
         <v>53</v>
@@ -4693,12 +4690,12 @@
         <v>52</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -4713,19 +4710,19 @@
         <v>0.2624750499002</v>
       </c>
       <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" t="s">
         <v>107</v>
       </c>
-      <c r="G39" t="s">
-        <v>108</v>
-      </c>
       <c r="H39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I39" t="n">
         <v>0.0708582834331337</v>
       </c>
       <c r="J39" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K39" t="s">
         <v>63</v>
@@ -4734,12 +4731,12 @@
         <v>62</v>
       </c>
       <c r="M39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -4754,19 +4751,19 @@
         <v>0.297948717948718</v>
       </c>
       <c r="F40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" t="s">
         <v>107</v>
       </c>
-      <c r="G40" t="s">
-        <v>108</v>
-      </c>
       <c r="H40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I40" t="n">
         <v>0.125128205128205</v>
       </c>
       <c r="J40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K40" t="s">
         <v>63</v>
@@ -4775,12 +4772,12 @@
         <v>62</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -4795,19 +4792,19 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
+        <v>131</v>
+      </c>
+      <c r="G41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" t="s">
         <v>132</v>
-      </c>
-      <c r="G41" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" t="s">
-        <v>133</v>
       </c>
       <c r="I41" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="J41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K41" t="s">
         <v>63</v>
@@ -4816,12 +4813,12 @@
         <v>62</v>
       </c>
       <c r="M41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -4836,19 +4833,19 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G42" t="s">
         <v>16</v>
       </c>
       <c r="H42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I42" t="n">
         <v>0.5</v>
       </c>
       <c r="J42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K42" t="s">
         <v>63</v>
@@ -4857,80 +4854,80 @@
         <v>62</v>
       </c>
       <c r="M42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" t="n">
         <v>0.1</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E43" t="n">
         <v>0.103980099502488</v>
       </c>
       <c r="F43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" t="s">
         <v>107</v>
       </c>
-      <c r="G43" t="s">
-        <v>108</v>
-      </c>
       <c r="H43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I43" t="n">
-        <v>0.00398009950248755</v>
+        <v>0.00398009950248761</v>
       </c>
       <c r="J43" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K43" t="s">
         <v>63</v>
       </c>
       <c r="L43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C44" t="n">
         <v>0.275862068965517</v>
       </c>
       <c r="D44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E44" t="n">
         <v>0.701734750979295</v>
       </c>
       <c r="F44" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H44" t="s">
         <v>217</v>
-      </c>
-      <c r="G44" t="s">
-        <v>126</v>
-      </c>
-      <c r="H44" t="s">
-        <v>218</v>
       </c>
       <c r="I44" t="n">
         <v>0.425872682013778</v>
       </c>
       <c r="J44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K44" t="s">
         <v>63</v>
@@ -4939,39 +4936,39 @@
         <v>68</v>
       </c>
       <c r="M44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C45" t="n">
         <v>0.275862068965517</v>
       </c>
       <c r="D45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E45" t="n">
         <v>0.625975473801561</v>
       </c>
       <c r="F45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I45" t="n">
         <v>0.350113404836043</v>
       </c>
       <c r="J45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K45" t="s">
         <v>63</v>
@@ -4980,12 +4977,12 @@
         <v>68</v>
       </c>
       <c r="M45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
         <v>27</v>
@@ -5000,19 +4997,19 @@
         <v>0.437233693870862</v>
       </c>
       <c r="F46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" t="s">
         <v>125</v>
-      </c>
-      <c r="G46" t="s">
-        <v>126</v>
-      </c>
-      <c r="H46" t="s">
-        <v>127</v>
       </c>
       <c r="I46" t="n">
         <v>0.271099639462471</v>
       </c>
       <c r="J46" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K46" t="s">
         <v>63</v>
@@ -5021,39 +5018,39 @@
         <v>64</v>
       </c>
       <c r="M46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C47" t="n">
         <v>0.375</v>
       </c>
       <c r="D47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E47" t="n">
         <v>0.601405405405405</v>
       </c>
       <c r="F47" t="s">
+        <v>199</v>
+      </c>
+      <c r="G47" t="s">
         <v>200</v>
       </c>
-      <c r="G47" t="s">
-        <v>201</v>
-      </c>
       <c r="H47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I47" t="n">
         <v>0.226405405405405</v>
       </c>
       <c r="J47" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K47" t="s">
         <v>63</v>
@@ -5062,39 +5059,39 @@
         <v>74</v>
       </c>
       <c r="M47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C48" t="n">
         <v>0.18</v>
       </c>
       <c r="D48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E48" t="n">
         <v>0.8800792864222</v>
       </c>
       <c r="F48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" t="s">
         <v>107</v>
       </c>
-      <c r="G48" t="s">
-        <v>108</v>
-      </c>
       <c r="H48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I48" t="n">
         <v>0.7000792864222</v>
       </c>
       <c r="J48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K48" t="s">
         <v>63</v>
@@ -5103,12 +5100,12 @@
         <v>74</v>
       </c>
       <c r="M48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
         <v>72</v>
@@ -5123,19 +5120,19 @@
         <v>0.75</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G49" t="s">
         <v>16</v>
       </c>
       <c r="H49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I49" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="J49" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K49" t="s">
         <v>63</v>
@@ -5144,258 +5141,258 @@
         <v>74</v>
       </c>
       <c r="M49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C50" t="n">
         <v>0.916666666666667</v>
       </c>
       <c r="D50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E50" t="n">
         <v>0.516666666666667</v>
       </c>
       <c r="F50" t="s">
+        <v>229</v>
+      </c>
+      <c r="G50" t="s">
+        <v>124</v>
+      </c>
+      <c r="H50" t="s">
         <v>230</v>
-      </c>
-      <c r="G50" t="s">
-        <v>126</v>
-      </c>
-      <c r="H50" t="s">
-        <v>231</v>
       </c>
       <c r="I50" t="n">
         <v>0.4</v>
       </c>
       <c r="J50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K50" t="s">
         <v>77</v>
       </c>
       <c r="L50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C51" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="D51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E51" t="n">
         <v>0.684210526315789</v>
       </c>
       <c r="F51" t="s">
+        <v>186</v>
+      </c>
+      <c r="G51" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" t="s">
         <v>187</v>
-      </c>
-      <c r="G51" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" t="s">
-        <v>188</v>
       </c>
       <c r="I51" t="n">
         <v>0.398496240601504</v>
       </c>
       <c r="J51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K51" t="s">
         <v>81</v>
       </c>
       <c r="L51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C52" t="n">
         <v>0.325</v>
       </c>
       <c r="D52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E52" t="n">
         <v>0.585404094581808</v>
       </c>
       <c r="F52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G52" t="s">
         <v>16</v>
       </c>
       <c r="H52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I52" t="n">
         <v>0.260404094581808</v>
       </c>
       <c r="J52" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K52" t="s">
         <v>81</v>
       </c>
       <c r="L52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C53" t="n">
         <v>0.325</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" t="n">
         <v>0.512010394761587</v>
       </c>
       <c r="F53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G53" t="s">
         <v>16</v>
       </c>
       <c r="H53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I53" t="n">
         <v>0.187010394761587</v>
       </c>
       <c r="J53" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K53" t="s">
         <v>81</v>
       </c>
       <c r="L53" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C54" t="n">
         <v>0.175</v>
       </c>
       <c r="D54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E54" t="n">
         <v>0.878848063555114</v>
       </c>
       <c r="F54" t="s">
+        <v>106</v>
+      </c>
+      <c r="G54" t="s">
         <v>107</v>
       </c>
-      <c r="G54" t="s">
-        <v>108</v>
-      </c>
       <c r="H54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I54" t="n">
         <v>0.703848063555114</v>
       </c>
       <c r="J54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K54" t="s">
         <v>81</v>
       </c>
       <c r="L54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C55" t="n">
         <v>0.15</v>
       </c>
       <c r="D55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E55" t="n">
         <v>0.878848063555114</v>
       </c>
       <c r="F55" t="s">
+        <v>106</v>
+      </c>
+      <c r="G55" t="s">
         <v>107</v>
       </c>
-      <c r="G55" t="s">
-        <v>108</v>
-      </c>
       <c r="H55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I55" t="n">
         <v>0.728848063555114</v>
       </c>
       <c r="J55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K55" t="s">
         <v>81</v>
       </c>
       <c r="L55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
@@ -5410,19 +5407,19 @@
         <v>0.135135135135135</v>
       </c>
       <c r="F56" t="s">
+        <v>106</v>
+      </c>
+      <c r="G56" t="s">
         <v>107</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>108</v>
-      </c>
-      <c r="H56" t="s">
-        <v>109</v>
       </c>
       <c r="I56" t="n">
         <v>0.142642642642643</v>
       </c>
       <c r="J56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K56" t="s">
         <v>81</v>
@@ -5431,12 +5428,12 @@
         <v>80</v>
       </c>
       <c r="M56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
         <v>78</v>
@@ -5451,19 +5448,19 @@
         <v>0.605815347721823</v>
       </c>
       <c r="F57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I57" t="n">
         <v>0.172482014388489</v>
       </c>
       <c r="J57" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K57" t="s">
         <v>81</v>
@@ -5472,53 +5469,53 @@
         <v>80</v>
       </c>
       <c r="M57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C58" t="n">
         <v>0.529411764705882</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E58" t="n">
         <v>0.17979797979798</v>
       </c>
       <c r="F58" t="s">
+        <v>106</v>
+      </c>
+      <c r="G58" t="s">
         <v>107</v>
       </c>
-      <c r="G58" t="s">
-        <v>108</v>
-      </c>
       <c r="H58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I58" t="n">
         <v>0.349613784907903</v>
       </c>
       <c r="J58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K58" t="s">
         <v>81</v>
       </c>
       <c r="L58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
         <v>88</v>
@@ -5533,19 +5530,19 @@
         <v>0.126121635094716</v>
       </c>
       <c r="F59" t="s">
+        <v>106</v>
+      </c>
+      <c r="G59" t="s">
         <v>107</v>
       </c>
-      <c r="G59" t="s">
-        <v>108</v>
-      </c>
       <c r="H59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I59" t="n">
         <v>0.311378364905284</v>
       </c>
       <c r="J59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K59" t="s">
         <v>83</v>
@@ -5554,12 +5551,12 @@
         <v>85</v>
       </c>
       <c r="M59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
         <v>47</v>
@@ -5574,19 +5571,19 @@
         <v>0.611451942740286</v>
       </c>
       <c r="F60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I60" t="n">
         <v>0.201048057259714</v>
       </c>
       <c r="J60" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K60" t="s">
         <v>83</v>
@@ -5595,12 +5592,12 @@
         <v>85</v>
       </c>
       <c r="M60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
         <v>90</v>
@@ -5615,19 +5612,19 @@
         <v>0.924317209608424</v>
       </c>
       <c r="F61" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" t="s">
         <v>107</v>
       </c>
-      <c r="G61" t="s">
-        <v>108</v>
-      </c>
       <c r="H61" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I61" t="n">
         <v>0.34098387627509</v>
       </c>
       <c r="J61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K61" t="s">
         <v>83</v>
@@ -5636,12 +5633,12 @@
         <v>92</v>
       </c>
       <c r="M61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
         <v>78</v>
@@ -5656,19 +5653,19 @@
         <v>0.605815347721823</v>
       </c>
       <c r="F62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I62" t="n">
         <v>0.172482014388489</v>
       </c>
       <c r="J62" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K62" t="s">
         <v>83</v>
@@ -5677,12 +5674,12 @@
         <v>82</v>
       </c>
       <c r="M62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
@@ -5697,19 +5694,19 @@
         <v>0.135135135135135</v>
       </c>
       <c r="F63" t="s">
+        <v>106</v>
+      </c>
+      <c r="G63" t="s">
         <v>107</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>108</v>
-      </c>
-      <c r="H63" t="s">
-        <v>109</v>
       </c>
       <c r="I63" t="n">
         <v>0.142642642642643</v>
       </c>
       <c r="J63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K63" t="s">
         <v>83</v>
@@ -5718,53 +5715,53 @@
         <v>82</v>
       </c>
       <c r="M63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C64" t="n">
         <v>0.517857142857143</v>
       </c>
       <c r="D64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E64" t="n">
         <v>0.772727272727273</v>
       </c>
       <c r="F64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I64" t="n">
         <v>0.25487012987013</v>
       </c>
       <c r="J64" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K64" t="s">
         <v>83</v>
       </c>
       <c r="L64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
         <v>86</v>
@@ -5779,19 +5776,19 @@
         <v>0.75</v>
       </c>
       <c r="F65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G65" t="s">
         <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I65" t="n">
         <v>0.146551724137931</v>
       </c>
       <c r="J65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K65" t="s">
         <v>83</v>
@@ -5800,135 +5797,135 @@
         <v>87</v>
       </c>
       <c r="M65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C66" t="n">
         <v>0.310344827586207</v>
       </c>
       <c r="D66" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E66" t="n">
         <v>0.577236791447681</v>
       </c>
       <c r="F66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G66" t="s">
         <v>16</v>
       </c>
       <c r="H66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I66" t="n">
         <v>0.266891963861474</v>
       </c>
       <c r="J66" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K66" t="s">
         <v>83</v>
       </c>
       <c r="L66" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C67" t="n">
         <v>0.375</v>
       </c>
       <c r="D67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E67" t="n">
         <v>0.650154154940026</v>
       </c>
       <c r="F67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G67" t="s">
         <v>16</v>
       </c>
       <c r="H67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I67" t="n">
         <v>0.275154154940026</v>
       </c>
       <c r="J67" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K67" t="s">
         <v>20</v>
       </c>
       <c r="L67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C68" t="n">
         <v>0.452380952380952</v>
       </c>
       <c r="D68" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E68" t="n">
         <v>0.527603451343405</v>
       </c>
       <c r="F68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G68" t="s">
         <v>16</v>
       </c>
       <c r="H68" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I68" t="n">
         <v>0.0752224989624526</v>
       </c>
       <c r="J68" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K68" t="s">
         <v>20</v>
       </c>
       <c r="L68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
         <v>13</v>
@@ -5937,25 +5934,25 @@
         <v>0.333333333333333</v>
       </c>
       <c r="D69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E69" t="n">
         <v>0.521990601741349</v>
       </c>
       <c r="F69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G69" t="s">
         <v>16</v>
       </c>
       <c r="H69" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I69" t="n">
         <v>0.188657268408016</v>
       </c>
       <c r="J69" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K69" t="s">
         <v>20</v>
@@ -5964,12 +5961,12 @@
         <v>19</v>
       </c>
       <c r="M69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
@@ -5978,25 +5975,25 @@
         <v>0.565217391304348</v>
       </c>
       <c r="D70" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E70" t="n">
         <v>0.463517890772128</v>
       </c>
       <c r="F70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G70" t="s">
         <v>16</v>
       </c>
       <c r="H70" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I70" t="n">
         <v>0.10169950053222</v>
       </c>
       <c r="J70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K70" t="s">
         <v>20</v>
@@ -6005,53 +6002,53 @@
         <v>24</v>
       </c>
       <c r="M70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C71" t="n">
         <v>0.30952380952381</v>
       </c>
       <c r="D71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E71" t="n">
         <v>0.521990601741349</v>
       </c>
       <c r="F71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G71" t="s">
         <v>16</v>
       </c>
       <c r="H71" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I71" t="n">
         <v>0.21246679221754</v>
       </c>
       <c r="J71" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
       </c>
       <c r="L71" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>61</v>
@@ -6060,25 +6057,25 @@
         <v>0.461538461538462</v>
       </c>
       <c r="D72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E72" t="n">
         <v>0.575451847051682</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G72" t="s">
         <v>16</v>
       </c>
       <c r="H72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I72" t="n">
         <v>0.11391338551322</v>
       </c>
       <c r="J72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K72" t="s">
         <v>20</v>
@@ -6087,12 +6084,12 @@
         <v>19</v>
       </c>
       <c r="M72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
         <v>40</v>
@@ -6101,39 +6098,39 @@
         <v>0.438775510204082</v>
       </c>
       <c r="D73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E73" t="n">
         <v>0.58516202736899</v>
       </c>
       <c r="F73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G73" t="s">
         <v>16</v>
       </c>
       <c r="H73" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I73" t="n">
         <v>0.146386517164908</v>
       </c>
       <c r="J73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K73" t="s">
         <v>44</v>
       </c>
       <c r="L73" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
         <v>46</v>
@@ -6142,39 +6139,39 @@
         <v>0.54</v>
       </c>
       <c r="D74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E74" t="n">
         <v>0.578550689177066</v>
       </c>
       <c r="F74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G74" t="s">
         <v>16</v>
       </c>
       <c r="H74" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I74" t="n">
         <v>0.0385506891770656</v>
       </c>
       <c r="J74" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K74" t="s">
         <v>44</v>
       </c>
       <c r="L74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>42</v>
@@ -6183,39 +6180,39 @@
         <v>0.706666666666667</v>
       </c>
       <c r="D75" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E75" t="n">
         <v>0.488441145281018</v>
       </c>
       <c r="F75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G75" t="s">
         <v>16</v>
       </c>
       <c r="H75" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I75" t="n">
         <v>0.218225521385649</v>
       </c>
       <c r="J75" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K75" t="s">
         <v>44</v>
       </c>
       <c r="L75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M75" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>37</v>
@@ -6224,25 +6221,25 @@
         <v>0.277777777777778</v>
       </c>
       <c r="D76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E76" t="n">
         <v>0.75</v>
       </c>
       <c r="F76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G76" t="s">
         <v>16</v>
       </c>
       <c r="H76" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I76" t="n">
         <v>0.472222222222222</v>
       </c>
       <c r="J76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K76" t="s">
         <v>20</v>
@@ -6251,56 +6248,56 @@
         <v>39</v>
       </c>
       <c r="M76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C77" t="n">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E77" t="n">
         <v>0.75</v>
       </c>
       <c r="F77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G77" t="s">
         <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I77" t="n">
         <v>0.25</v>
       </c>
       <c r="J77" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K77" t="s">
         <v>63</v>
       </c>
       <c r="L77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C78" t="n">
         <v>0.82</v>
@@ -6312,33 +6309,33 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G78" t="s">
         <v>16</v>
       </c>
       <c r="H78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I78" t="n">
         <v>0.18</v>
       </c>
       <c r="J78" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K78" t="s">
         <v>63</v>
       </c>
       <c r="L78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B79" t="s">
         <v>69</v>
@@ -6347,25 +6344,25 @@
         <v>0.466666666666667</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E79" t="n">
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G79" t="s">
         <v>16</v>
       </c>
       <c r="H79" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I79" t="n">
         <v>0.533333333333333</v>
       </c>
       <c r="J79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K79" t="s">
         <v>63</v>
@@ -6374,53 +6371,53 @@
         <v>62</v>
       </c>
       <c r="M79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C80" t="n">
         <v>0.183673469387755</v>
       </c>
       <c r="D80" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E80" t="n">
         <v>0.5</v>
       </c>
       <c r="F80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G80" t="s">
         <v>16</v>
       </c>
       <c r="H80" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I80" t="n">
         <v>0.316326530612245</v>
       </c>
       <c r="J80" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K80" t="s">
         <v>44</v>
       </c>
       <c r="L80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
         <v>72</v>
@@ -6435,19 +6432,19 @@
         <v>0.75</v>
       </c>
       <c r="F81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G81" t="s">
         <v>16</v>
       </c>
       <c r="H81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I81" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="J81" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K81" t="s">
         <v>63</v>
@@ -6456,121 +6453,121 @@
         <v>74</v>
       </c>
       <c r="M81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B82" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C82" t="n">
         <v>0.14</v>
       </c>
       <c r="D82" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E82" t="n">
         <v>0.5</v>
       </c>
       <c r="F82" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G82" t="s">
         <v>16</v>
       </c>
       <c r="H82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I82" t="n">
         <v>0.36</v>
       </c>
       <c r="J82" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K82" t="s">
         <v>63</v>
       </c>
       <c r="L82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C83" t="n">
         <v>0.1</v>
       </c>
       <c r="D83" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E83" t="n">
         <v>0.5</v>
       </c>
       <c r="F83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G83" t="s">
         <v>16</v>
       </c>
       <c r="H83" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I83" t="n">
         <v>0.4</v>
       </c>
       <c r="J83" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K83" t="s">
         <v>63</v>
       </c>
       <c r="L83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B84" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C84" t="n">
         <v>0.87037037037037</v>
       </c>
       <c r="D84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E84" t="n">
         <v>0.620373134328358</v>
       </c>
       <c r="F84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G84" t="s">
         <v>16</v>
       </c>
       <c r="H84" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I84" t="n">
         <v>0.249997236042012</v>
       </c>
       <c r="J84" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="K84" t="s">
         <v>20</v>
@@ -6579,53 +6576,53 @@
         <v>39</v>
       </c>
       <c r="M84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B85" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C85" t="n">
         <v>0.346153846153846</v>
       </c>
       <c r="D85" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E85" t="n">
         <v>0.64430607966457</v>
       </c>
       <c r="F85" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G85" t="s">
         <v>16</v>
       </c>
       <c r="H85" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I85" t="n">
         <v>0.298152233510724</v>
       </c>
       <c r="J85" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K85" t="s">
         <v>20</v>
       </c>
       <c r="L85" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B86" t="s">
         <v>21</v>
@@ -6634,25 +6631,25 @@
         <v>0.565217391304348</v>
       </c>
       <c r="D86" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E86" t="n">
         <v>0.697544916081404</v>
       </c>
       <c r="F86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G86" t="s">
         <v>16</v>
       </c>
       <c r="H86" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I86" t="n">
         <v>0.132327524777056</v>
       </c>
       <c r="J86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K86" t="s">
         <v>20</v>
@@ -6661,7 +6658,7 @@
         <v>24</v>
       </c>
       <c r="M86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>